<commit_message>
Merged PR 7403: PRI-22572 Program Lineup Report- Accuracy Estimate Date data wraps to next line & hidden
PRI-22572 Bug fix and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED9D06CB-3320-47BA-9700-77344E35063E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
     <sheet name="Allocations" sheetId="6" r:id="rId2"/>
     <sheet name="Detailed View" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mgMtMfamHb1jVya39tpwhGUN2dNvA=="/>
@@ -102,11 +107,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -408,27 +413,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -467,9 +451,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Header" xfId="1"/>
+    <cellStyle name="Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
@@ -688,13 +693,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="1">
+    <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="28"/>
     </tableStyle>
-    <tableStyle name="Table Style 2" pivot="0" count="1">
+    <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="firstRowStripe" dxfId="27"/>
     </tableStyle>
-    <tableStyle name="Table Style 3" pivot="0" count="1">
+    <tableStyle name="Table Style 3" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="firstRowStripe" dxfId="26"/>
     </tableStyle>
   </tableStyles>
@@ -733,7 +738,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31D95EB8-DCD9-2744-84D9-02A9C5C5940A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D95EB8-DCD9-2744-84D9-02A9C5C5940A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -771,7 +776,7 @@
         <xdr:cNvPr id="3" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AF06897-AADC-DE4F-8E7F-8EC6B650C447}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF06897-AADC-DE4F-8E7F-8EC6B650C447}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -809,7 +814,7 @@
         <xdr:cNvPr id="4" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5C4D1073-2405-0E40-AFA9-1588F00557C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4D1073-2405-0E40-AFA9-1588F00557C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -852,7 +857,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C7340664-924A-A749-A299-ABFED4F695AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7340664-924A-A749-A299-ABFED4F695AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -890,7 +895,7 @@
         <xdr:cNvPr id="3" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ADB4D162-0877-9F4E-A6D6-0A3AD2F37961}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADB4D162-0877-9F4E-A6D6-0A3AD2F37961}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -933,7 +938,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1158,32 +1163,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="22" customWidth="1"/>
     <col min="6" max="6" width="18" style="22" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="22" customWidth="1"/>
     <col min="8" max="8" width="28" style="22" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.77734375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="22" customWidth="1"/>
-    <col min="13" max="16384" width="14.44140625" style="22"/>
+    <col min="9" max="9" width="13.28515625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="22" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="39" customHeight="1">
+    <row r="2" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1195,29 +1200,29 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2"/>
-      <c r="I2" s="34">
+      <c r="I2" s="50">
         <f>'Detailed View'!I2:J2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="20"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="16.05" customHeight="1">
+    <row r="3" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="16.05" customHeight="1">
+    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="23"/>
@@ -1231,11 +1236,11 @@
       <c r="K4" s="18"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1259,21 +1264,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1">
-      <c r="B6" s="32">
+    <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="46">
         <f>'Detailed View'!B6:C6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="25">
         <f>'Detailed View'!D6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="47">
         <f>'Detailed View'!E6:F6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="25">
         <f>'Detailed View'!G6</f>
         <v>0</v>
@@ -1296,7 +1301,7 @@
       </c>
       <c r="L6" s="25"/>
     </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1">
+    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
@@ -1319,20 +1324,20 @@
       <c r="J8"/>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="9" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="50"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="43"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="10" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -1345,7 +1350,7 @@
       <c r="J10"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="11" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -1358,7 +1363,7 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="12" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -1371,7 +1376,7 @@
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="13" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -1384,7 +1389,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="14" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -1397,7 +1402,7 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="15" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -1410,7 +1415,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="16" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1423,7 +1428,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="17" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1436,7 +1441,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="18" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1449,7 +1454,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="19" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1462,7 +1467,7 @@
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="20" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1475,7 +1480,7 @@
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="21" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1488,7 +1493,7 @@
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="22" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1501,7 +1506,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="23" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1514,7 +1519,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="24" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1527,7 +1532,7 @@
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="25" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -1540,7 +1545,7 @@
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="26" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -1553,7 +1558,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="27" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -1566,7 +1571,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="28" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -1579,7 +1584,7 @@
       <c r="J28"/>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="29" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -1592,7 +1597,7 @@
       <c r="J29"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -1605,320 +1610,320 @@
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="31" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="32" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="33" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="34" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
     </row>
-    <row r="35" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="35" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="36" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="37" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="38" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="39" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
     </row>
-    <row r="40" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="40" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="41" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="43" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="44" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="45" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="46" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="47" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="48" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="49" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="50" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
     </row>
-    <row r="51" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="51" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
     </row>
-    <row r="52" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="52" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="53" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="54" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="55" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="56" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="57" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="58" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="59" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="60" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="61" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="62" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="63" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="64" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="65" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="66" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="67" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="68" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="69" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="70" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="71" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
     </row>
-    <row r="72" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="72" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
     </row>
-    <row r="73" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="73" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
     </row>
-    <row r="74" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="74" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
     </row>
-    <row r="75" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="75" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
     </row>
-    <row r="76" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="76" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
     </row>
-    <row r="77" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="77" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
     </row>
-    <row r="78" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="78" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
     </row>
-    <row r="79" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="79" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
     </row>
-    <row r="80" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="80" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
     </row>
-    <row r="81" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="81" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
     </row>
-    <row r="82" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="82" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
     </row>
-    <row r="83" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="83" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
     </row>
-    <row r="84" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="84" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
     </row>
-    <row r="85" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="85" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
     </row>
-    <row r="86" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="86" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
     </row>
-    <row r="87" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="87" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
     </row>
-    <row r="88" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="88" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
     </row>
-    <row r="89" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="89" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
     </row>
-    <row r="90" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="90" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
     </row>
-    <row r="91" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="91" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
     </row>
-    <row r="92" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="92" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
     </row>
-    <row r="93" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="93" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
     </row>
-    <row r="94" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="94" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
     </row>
-    <row r="95" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="95" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
     </row>
-    <row r="96" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="96" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
     </row>
-    <row r="97" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="97" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
     </row>
-    <row r="98" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="98" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
     </row>
-    <row r="99" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="99" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
     </row>
-    <row r="100" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="100" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
     </row>
-    <row r="101" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="101" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
     </row>
-    <row r="102" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="102" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
     </row>
-    <row r="103" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="103" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="10:11" ht="15" customHeight="1">
+    <row r="104" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="10:11" ht="15" customHeight="1">
+    <row r="105" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J105" s="7"/>
     </row>
-    <row r="106" spans="10:11" ht="15" customHeight="1">
+    <row r="106" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J106" s="7"/>
     </row>
-    <row r="107" spans="10:11" ht="15" customHeight="1">
+    <row r="107" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J107" s="7"/>
     </row>
-    <row r="108" spans="10:11" ht="15" customHeight="1">
+    <row r="108" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="10:11" ht="15" customHeight="1">
+    <row r="109" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J109" s="7"/>
     </row>
-    <row r="110" spans="10:11" ht="15" customHeight="1">
+    <row r="110" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J110" s="7"/>
     </row>
-    <row r="111" spans="10:11" ht="15" customHeight="1">
+    <row r="111" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J111" s="7"/>
     </row>
   </sheetData>
@@ -1933,42 +1938,42 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="7" priority="21">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:D8">
-    <cfRule type="expression" dxfId="6" priority="19">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>$A8="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="5" priority="18">
+    <cfRule type="expression" dxfId="23" priority="18">
       <formula>$A8="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="4" priority="17">
+    <cfRule type="expression" dxfId="22" priority="17">
       <formula>$A8="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="3" priority="16">
+    <cfRule type="expression" dxfId="21" priority="16">
       <formula>$A8="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="2" priority="15">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>$A8="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$A3="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1979,32 +1984,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:L105"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="22" customWidth="1"/>
     <col min="8" max="8" width="28" style="22" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.77734375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="22" customWidth="1"/>
-    <col min="13" max="16384" width="14.44140625" style="22"/>
+    <col min="9" max="9" width="13.28515625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="22" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="39" customHeight="1">
+    <row r="2" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2016,29 +2021,29 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2"/>
-      <c r="I2" s="34">
+      <c r="I2" s="50">
         <f>'Detailed View'!I2:J2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="20"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="16.05" customHeight="1">
+    <row r="3" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="16.05" customHeight="1">
+    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="23"/>
@@ -2052,11 +2057,11 @@
       <c r="K4" s="18"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
@@ -2080,21 +2085,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1">
-      <c r="B6" s="32">
+    <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="46">
         <f>'Detailed View'!B6:C6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="25">
         <f>'Detailed View'!D6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="47">
         <f>'Detailed View'!E6:F6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="25">
         <f>'Detailed View'!G6</f>
         <v>0</v>
@@ -2117,15 +2122,15 @@
       </c>
       <c r="L6" s="25"/>
     </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1"/>
-    <row r="9" spans="1:12" customFormat="1" ht="24" customHeight="1">
-      <c r="B9" s="35" t="s">
+    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-    </row>
-    <row r="10" spans="1:12" customFormat="1" ht="24" customHeight="1">
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
         <v>6</v>
@@ -2134,24 +2139,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" customFormat="1" ht="24" customHeight="1">
-      <c r="B11" s="47"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-    </row>
-    <row r="12" spans="1:12" customFormat="1" ht="24" customHeight="1">
+    <row r="11" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:12" customFormat="1" ht="24" customHeight="1">
-      <c r="B13" s="35" t="s">
+    <row r="13" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-    </row>
-    <row r="14" spans="1:12" customFormat="1" ht="24" customHeight="1">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+    </row>
+    <row r="14" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
         <v>7</v>
@@ -2160,24 +2165,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" customFormat="1" ht="24" customHeight="1">
-      <c r="B15" s="42"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="43"/>
-    </row>
-    <row r="16" spans="1:12" customFormat="1" ht="24" customHeight="1">
+    <row r="15" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="36"/>
+    </row>
+    <row r="16" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
     </row>
-    <row r="17" spans="2:4" customFormat="1" ht="24" customHeight="1">
-      <c r="B17" s="36" t="s">
+    <row r="17" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-    </row>
-    <row r="18" spans="2:4" customFormat="1" ht="24" customHeight="1">
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+    </row>
+    <row r="18" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
         <v>0</v>
@@ -2186,156 +2191,156 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:4" customFormat="1" ht="24" customHeight="1">
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
-    </row>
-    <row r="20" spans="2:4" customFormat="1" ht="24" customHeight="1"/>
-    <row r="21" spans="2:4" customFormat="1" ht="24" customHeight="1"/>
-    <row r="22" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="23" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="24" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="25" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="26" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="27" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="28" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="29" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="30" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="31" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="32" spans="2:4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="33" customFormat="1" ht="15" customHeight="1"/>
-    <row r="34" customFormat="1" ht="15" customHeight="1"/>
-    <row r="35" customFormat="1" ht="15" customHeight="1"/>
-    <row r="36" customFormat="1" ht="15" customHeight="1"/>
-    <row r="37" customFormat="1" ht="15" customHeight="1"/>
-    <row r="38" customFormat="1" ht="15" customHeight="1"/>
-    <row r="39" customFormat="1" ht="15" customHeight="1"/>
-    <row r="40" customFormat="1" ht="15" customHeight="1"/>
-    <row r="41" customFormat="1" ht="15" customHeight="1"/>
-    <row r="42" customFormat="1" ht="15" customHeight="1"/>
-    <row r="43" customFormat="1" ht="15" customHeight="1"/>
-    <row r="44" customFormat="1" ht="15" customHeight="1"/>
-    <row r="45" customFormat="1" ht="15" customHeight="1"/>
-    <row r="46" customFormat="1" ht="15" customHeight="1"/>
-    <row r="47" customFormat="1" ht="15" customHeight="1"/>
-    <row r="48" customFormat="1" ht="15" customHeight="1"/>
-    <row r="49" customFormat="1" ht="15" customHeight="1"/>
-    <row r="50" customFormat="1" ht="15" customHeight="1"/>
-    <row r="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="52" customFormat="1" ht="15" customHeight="1"/>
-    <row r="53" customFormat="1" ht="15" customHeight="1"/>
-    <row r="54" customFormat="1" ht="15" customHeight="1"/>
-    <row r="55" customFormat="1" ht="15" customHeight="1"/>
-    <row r="56" customFormat="1" ht="15" customHeight="1"/>
-    <row r="57" customFormat="1" ht="15" customHeight="1"/>
-    <row r="58" customFormat="1" ht="15" customHeight="1"/>
-    <row r="59" customFormat="1" ht="15" customHeight="1"/>
-    <row r="60" customFormat="1" ht="15" customHeight="1"/>
-    <row r="61" customFormat="1" ht="15" customHeight="1"/>
-    <row r="62" customFormat="1" ht="15" customHeight="1"/>
-    <row r="63" customFormat="1" ht="15" customHeight="1"/>
-    <row r="64" customFormat="1" ht="15" customHeight="1"/>
-    <row r="65" customFormat="1" ht="15" customHeight="1"/>
-    <row r="66" customFormat="1" ht="15" customHeight="1"/>
-    <row r="67" customFormat="1" ht="15" customHeight="1"/>
-    <row r="68" customFormat="1" ht="15" customHeight="1"/>
-    <row r="69" customFormat="1" ht="15" customHeight="1"/>
-    <row r="70" customFormat="1" ht="15" customHeight="1"/>
-    <row r="71" customFormat="1" ht="15" customHeight="1"/>
-    <row r="72" customFormat="1" ht="15" customHeight="1"/>
-    <row r="73" customFormat="1" ht="15" customHeight="1"/>
-    <row r="74" customFormat="1" ht="15" customHeight="1"/>
-    <row r="75" customFormat="1" ht="15" customHeight="1"/>
-    <row r="76" customFormat="1" ht="15" customHeight="1"/>
-    <row r="77" customFormat="1" ht="15" customHeight="1"/>
-    <row r="78" customFormat="1" ht="15" customHeight="1"/>
-    <row r="79" customFormat="1" ht="15" customHeight="1"/>
-    <row r="80" customFormat="1" ht="15" customHeight="1"/>
-    <row r="81" spans="10:11" customFormat="1" ht="15" customHeight="1"/>
-    <row r="82" spans="10:11" customFormat="1" ht="15" customHeight="1"/>
-    <row r="83" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="19" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="10:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="10:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
     </row>
-    <row r="84" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="84" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
     </row>
-    <row r="85" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="85" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
     </row>
-    <row r="86" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="86" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
     </row>
-    <row r="87" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="87" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
     </row>
-    <row r="88" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="88" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
     </row>
-    <row r="89" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="89" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
     </row>
-    <row r="90" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="90" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
     </row>
-    <row r="91" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="91" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
     </row>
-    <row r="92" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="92" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
     </row>
-    <row r="93" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="93" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
     </row>
-    <row r="94" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="94" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
     </row>
-    <row r="95" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="95" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
     </row>
-    <row r="96" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="96" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
     </row>
-    <row r="97" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="97" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
     </row>
-    <row r="98" spans="10:11" ht="15" customHeight="1">
+    <row r="98" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J98" s="7"/>
     </row>
-    <row r="99" spans="10:11" ht="15" customHeight="1">
+    <row r="99" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J99" s="7"/>
     </row>
-    <row r="100" spans="10:11" ht="15" customHeight="1">
+    <row r="100" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J100" s="7"/>
     </row>
-    <row r="101" spans="10:11" ht="15" customHeight="1">
+    <row r="101" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J101" s="7"/>
     </row>
-    <row r="102" spans="10:11" ht="15" customHeight="1">
+    <row r="102" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J102" s="7"/>
     </row>
-    <row r="103" spans="10:11" ht="15" customHeight="1">
+    <row r="103" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J103" s="7"/>
     </row>
-    <row r="104" spans="10:11" ht="15" customHeight="1">
+    <row r="104" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="10:11" ht="15" customHeight="1">
+    <row r="105" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J105" s="7"/>
     </row>
   </sheetData>
@@ -2350,77 +2355,77 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="22" priority="19">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>$A13="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="20" priority="17">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>$A10="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="19" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>$A10="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>$A10="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="17" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>$A16="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>$A9="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>$A17="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>$A17="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>$A17="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>$A3="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2431,36 +2436,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" customWidth="1"/>
-    <col min="11" max="11" width="19.77734375" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:14" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1">
+    <row r="2" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2471,46 +2476,46 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="20"/>
       <c r="L2" s="1"/>
       <c r="N2" s="22"/>
     </row>
-    <row r="3" spans="1:14" ht="16.05" customHeight="1">
+    <row r="3" spans="1:14" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="N3" s="22"/>
     </row>
-    <row r="4" spans="1:14" ht="16.05" customHeight="1">
+    <row r="4" spans="1:14" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:14" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:14" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="19" t="s">
         <v>13</v>
       </c>
@@ -2534,12 +2539,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="15" customFormat="1" ht="18" customHeight="1">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+    <row r="6" spans="1:14" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="16"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -2547,7 +2552,7 @@
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
     </row>
-    <row r="8" spans="1:14" ht="24" customHeight="1">
+    <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="10" t="s">
         <v>10</v>
@@ -2578,20 +2583,20 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:14" s="24" customFormat="1" ht="24" customHeight="1">
+    <row r="9" spans="1:14" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="37"/>
-    </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -2603,328 +2608,328 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="15" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="17" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="19" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="23" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="24" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
     </row>
-    <row r="25" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="25" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="26" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="27" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="28" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="29" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="31" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="32" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="33" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="34" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
     </row>
-    <row r="35" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="35" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="36" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="37" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="38" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="39" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
     </row>
-    <row r="40" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="40" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="41" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="43" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="44" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="45" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="46" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="47" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="48" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="49" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="50" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
     </row>
-    <row r="51" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="51" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
     </row>
-    <row r="52" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="52" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="53" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="54" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="55" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="56" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="57" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="58" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="59" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="60" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="61" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="62" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="63" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="64" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="65" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="66" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="67" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="68" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="69" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="70" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="71" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
     </row>
-    <row r="72" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="72" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
     </row>
-    <row r="73" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="73" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
     </row>
-    <row r="74" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="74" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
     </row>
-    <row r="75" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="75" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
     </row>
-    <row r="76" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="76" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
     </row>
-    <row r="77" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="77" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
     </row>
-    <row r="78" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="78" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
     </row>
-    <row r="79" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="79" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
     </row>
-    <row r="80" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="80" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
     </row>
-    <row r="81" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="81" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
     </row>
-    <row r="82" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="82" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
     </row>
-    <row r="83" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="83" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
     </row>
-    <row r="84" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="84" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
     </row>
-    <row r="85" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1">
+    <row r="85" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
     </row>
-    <row r="86" spans="10:11" ht="15" customHeight="1">
+    <row r="86" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J86" s="7"/>
     </row>
-    <row r="87" spans="10:11" ht="15" customHeight="1">
+    <row r="87" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J87" s="7"/>
     </row>
-    <row r="88" spans="10:11" ht="15" customHeight="1">
+    <row r="88" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J88" s="7"/>
     </row>
-    <row r="89" spans="10:11" ht="15" customHeight="1">
+    <row r="89" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J89" s="7"/>
     </row>
-    <row r="90" spans="10:11" ht="15" customHeight="1">
+    <row r="90" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J90" s="7"/>
     </row>
-    <row r="91" spans="10:11" ht="15" customHeight="1">
+    <row r="91" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J91" s="7"/>
     </row>
-    <row r="92" spans="10:11" ht="15" customHeight="1">
+    <row r="92" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J92" s="7"/>
     </row>
-    <row r="93" spans="10:11" ht="15" customHeight="1">
+    <row r="93" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J93" s="7"/>
     </row>
   </sheetData>
@@ -2937,17 +2942,17 @@
     <mergeCell ref="D3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="B8 B4">
-    <cfRule type="expression" dxfId="25" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A3="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2958,9 +2963,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3187,19 +3195,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3224,9 +3228,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 7427: PRI-22572 Program Lineup Report- Accuracy Estimate Date data wraps to next line & hidden
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED9D06CB-3320-47BA-9700-77344E35063E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{874CB67B-78D4-4FF4-A247-4B9D31C3B17E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
@@ -470,7 +470,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1166,9 +1166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L111"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2439,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
     </sheetView>
@@ -2963,15 +2963,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3194,21 +3185,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3227,11 +3219,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 7724: PRI-20082 Program Lineup Report - Default View tab - Lineup Listing Section
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{874CB67B-78D4-4FF4-A247-4B9D31C3B17E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2146642-CCAE-4614-8C51-0E4CC814A074}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,84 +463,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -694,13 +631,13 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="28"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="27"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="26"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -727,7 +664,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -765,7 +702,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -803,7 +740,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -927,7 +864,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1164,125 +1101,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L111"/>
+  <dimension ref="A2:M111"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6:C6"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="18" style="22" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="28" style="22" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="22" customWidth="1"/>
-    <col min="13" max="16384" width="14.42578125" style="22"/>
+    <col min="1" max="1" width="3" style="22" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="18" style="22" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="28" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="22" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="22" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="22" customWidth="1"/>
+    <col min="14" max="16384" width="14.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="2:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="27" t="str">
-        <f>'Detailed View'!D2</f>
+      <c r="D2" s="1"/>
+      <c r="E2" s="27" t="str">
+        <f>'Detailed View'!E2</f>
         <v xml:space="preserve"> | Program Lineup*</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2"/>
-      <c r="I2" s="50">
-        <f>'Detailed View'!I2:J2</f>
+      <c r="H2" s="1"/>
+      <c r="I2"/>
+      <c r="J2" s="48">
+        <f>'Detailed View'!J2:K2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="D3" s="44" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="2:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="E3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="44"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
       <c r="I3" s="44"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="2:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="17"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="45"/>
+      <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="F5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
-        <f>'Detailed View'!B6:C6</f>
+    <row r="6" spans="2:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="46">
+        <f>'Detailed View'!C6:D6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="25">
-        <f>'Detailed View'!D6</f>
+      <c r="D6" s="46"/>
+      <c r="E6" s="25">
+        <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="47">
-        <f>'Detailed View'!E6:F6</f>
+      <c r="F6" s="47">
+        <f>'Detailed View'!F6:G6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="25">
-        <f>'Detailed View'!G6</f>
-        <v>0</v>
-      </c>
+      <c r="G6" s="47"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -1299,46 +1233,49 @@
         <f>'Detailed View'!K6</f>
         <v>0</v>
       </c>
-      <c r="L6" s="25"/>
-    </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
+      <c r="L6" s="25">
+        <f>'Detailed View'!L6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="25"/>
+    </row>
+    <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8"/>
+      <c r="I8" s="5"/>
       <c r="J8"/>
       <c r="K8"/>
-    </row>
-    <row r="9" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="32"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
-      <c r="H9" s="43"/>
-      <c r="I9"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="43"/>
       <c r="J9"/>
       <c r="K9"/>
-    </row>
-    <row r="10" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
@@ -1349,9 +1286,9 @@
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
-    </row>
-    <row r="11" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
@@ -1362,9 +1299,9 @@
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
-    </row>
-    <row r="12" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
@@ -1375,9 +1312,9 @@
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
-    </row>
-    <row r="13" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -1388,9 +1325,9 @@
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
-    </row>
-    <row r="14" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14"/>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -1401,9 +1338,9 @@
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
-    </row>
-    <row r="15" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15"/>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
@@ -1414,9 +1351,9 @@
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
-    </row>
-    <row r="16" spans="1:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16"/>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -1427,9 +1364,9 @@
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
-    </row>
-    <row r="17" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -1440,9 +1377,9 @@
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
-    </row>
-    <row r="18" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
@@ -1453,9 +1390,9 @@
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
-    </row>
-    <row r="19" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
@@ -1466,9 +1403,9 @@
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
-    </row>
-    <row r="20" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
@@ -1479,9 +1416,9 @@
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
-    </row>
-    <row r="21" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -1492,9 +1429,9 @@
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
-    </row>
-    <row r="22" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22"/>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
@@ -1505,9 +1442,9 @@
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
-    </row>
-    <row r="23" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
@@ -1518,9 +1455,9 @@
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
-    </row>
-    <row r="24" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24"/>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
@@ -1531,9 +1468,9 @@
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
-    </row>
-    <row r="25" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25"/>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -1544,9 +1481,9 @@
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
-    </row>
-    <row r="26" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26"/>
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -1557,9 +1494,9 @@
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
-    </row>
-    <row r="27" spans="1:11" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27"/>
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="2:12" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -1570,9 +1507,9 @@
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
-    </row>
-    <row r="28" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28"/>
+      <c r="L27"/>
+    </row>
+    <row r="28" spans="2:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -1583,9 +1520,9 @@
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
-    </row>
-    <row r="29" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29"/>
+      <c r="L28"/>
+    </row>
+    <row r="29" spans="2:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1596,9 +1533,9 @@
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
-    </row>
-    <row r="30" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30"/>
+      <c r="L29"/>
+    </row>
+    <row r="30" spans="2:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1609,372 +1546,338 @@
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
-    </row>
-    <row r="31" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J31" s="9"/>
+      <c r="L30"/>
+    </row>
+    <row r="31" spans="2:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J32" s="9"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="2:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="9"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J34" s="9"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K34" s="9"/>
-    </row>
-    <row r="35" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J35" s="9"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K35" s="9"/>
-    </row>
-    <row r="36" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J36" s="9"/>
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K36" s="9"/>
-    </row>
-    <row r="37" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J37" s="9"/>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J38" s="9"/>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K38" s="9"/>
-    </row>
-    <row r="39" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J39" s="9"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J40" s="9"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K40" s="9"/>
-    </row>
-    <row r="41" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J41" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K41" s="9"/>
-    </row>
-    <row r="42" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="9"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K42" s="9"/>
-    </row>
-    <row r="43" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J43" s="9"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K43" s="9"/>
-    </row>
-    <row r="44" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="9"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K44" s="9"/>
-    </row>
-    <row r="45" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J45" s="9"/>
+      <c r="L44" s="9"/>
+    </row>
+    <row r="45" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K45" s="9"/>
-    </row>
-    <row r="46" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J46" s="9"/>
+      <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K46" s="9"/>
-    </row>
-    <row r="47" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J47" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K47" s="9"/>
-    </row>
-    <row r="48" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J48" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K48" s="9"/>
-    </row>
-    <row r="49" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J49" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K49" s="9"/>
-    </row>
-    <row r="50" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J50" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K50" s="9"/>
-    </row>
-    <row r="51" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J51" s="9"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K51" s="9"/>
-    </row>
-    <row r="52" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J52" s="9"/>
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K52" s="9"/>
-    </row>
-    <row r="53" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J53" s="9"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K53" s="9"/>
-    </row>
-    <row r="54" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J54" s="9"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K54" s="9"/>
-    </row>
-    <row r="55" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J55" s="9"/>
+      <c r="L54" s="9"/>
+    </row>
+    <row r="55" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K55" s="9"/>
-    </row>
-    <row r="56" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J56" s="9"/>
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K56" s="9"/>
-    </row>
-    <row r="57" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J57" s="9"/>
+      <c r="L56" s="9"/>
+    </row>
+    <row r="57" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K57" s="9"/>
-    </row>
-    <row r="58" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J58" s="9"/>
+      <c r="L57" s="9"/>
+    </row>
+    <row r="58" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K58" s="9"/>
-    </row>
-    <row r="59" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J59" s="9"/>
+      <c r="L58" s="9"/>
+    </row>
+    <row r="59" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K59" s="9"/>
-    </row>
-    <row r="60" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J60" s="9"/>
+      <c r="L59" s="9"/>
+    </row>
+    <row r="60" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K60" s="9"/>
-    </row>
-    <row r="61" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J61" s="9"/>
+      <c r="L60" s="9"/>
+    </row>
+    <row r="61" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K61" s="9"/>
-    </row>
-    <row r="62" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J62" s="9"/>
+      <c r="L61" s="9"/>
+    </row>
+    <row r="62" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K62" s="9"/>
-    </row>
-    <row r="63" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J63" s="9"/>
+      <c r="L62" s="9"/>
+    </row>
+    <row r="63" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K63" s="9"/>
-    </row>
-    <row r="64" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J64" s="9"/>
+      <c r="L63" s="9"/>
+    </row>
+    <row r="64" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K64" s="9"/>
-    </row>
-    <row r="65" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J65" s="9"/>
+      <c r="L64" s="9"/>
+    </row>
+    <row r="65" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K65" s="9"/>
-    </row>
-    <row r="66" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J66" s="9"/>
+      <c r="L65" s="9"/>
+    </row>
+    <row r="66" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K66" s="9"/>
-    </row>
-    <row r="67" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J67" s="9"/>
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K67" s="9"/>
-    </row>
-    <row r="68" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J68" s="9"/>
+      <c r="L67" s="9"/>
+    </row>
+    <row r="68" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K68" s="9"/>
-    </row>
-    <row r="69" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J69" s="9"/>
+      <c r="L68" s="9"/>
+    </row>
+    <row r="69" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K69" s="9"/>
-    </row>
-    <row r="70" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J70" s="9"/>
+      <c r="L69" s="9"/>
+    </row>
+    <row r="70" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K70" s="9"/>
-    </row>
-    <row r="71" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J71" s="9"/>
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K71" s="9"/>
-    </row>
-    <row r="72" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J72" s="9"/>
+      <c r="L71" s="9"/>
+    </row>
+    <row r="72" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K72" s="9"/>
-    </row>
-    <row r="73" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J73" s="9"/>
+      <c r="L72" s="9"/>
+    </row>
+    <row r="73" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K73" s="9"/>
-    </row>
-    <row r="74" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J74" s="9"/>
+      <c r="L73" s="9"/>
+    </row>
+    <row r="74" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K74" s="9"/>
-    </row>
-    <row r="75" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J75" s="9"/>
+      <c r="L74" s="9"/>
+    </row>
+    <row r="75" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K75" s="9"/>
-    </row>
-    <row r="76" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J76" s="9"/>
+      <c r="L75" s="9"/>
+    </row>
+    <row r="76" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K76" s="9"/>
-    </row>
-    <row r="77" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J77" s="9"/>
+      <c r="L76" s="9"/>
+    </row>
+    <row r="77" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K77" s="9"/>
-    </row>
-    <row r="78" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J78" s="9"/>
+      <c r="L77" s="9"/>
+    </row>
+    <row r="78" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K78" s="9"/>
-    </row>
-    <row r="79" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="9"/>
+      <c r="L78" s="9"/>
+    </row>
+    <row r="79" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K79" s="9"/>
-    </row>
-    <row r="80" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="9"/>
+      <c r="L79" s="9"/>
+    </row>
+    <row r="80" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K80" s="9"/>
-    </row>
-    <row r="81" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="9"/>
+      <c r="L80" s="9"/>
+    </row>
+    <row r="81" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K81" s="9"/>
-    </row>
-    <row r="82" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="9"/>
+      <c r="L81" s="9"/>
+    </row>
+    <row r="82" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K82" s="9"/>
-    </row>
-    <row r="83" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="9"/>
+      <c r="L82" s="9"/>
+    </row>
+    <row r="83" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K83" s="9"/>
-    </row>
-    <row r="84" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="9"/>
+      <c r="L83" s="9"/>
+    </row>
+    <row r="84" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K84" s="9"/>
-    </row>
-    <row r="85" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="9"/>
+      <c r="L84" s="9"/>
+    </row>
+    <row r="85" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K85" s="9"/>
-    </row>
-    <row r="86" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="9"/>
+      <c r="L85" s="9"/>
+    </row>
+    <row r="86" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K86" s="9"/>
-    </row>
-    <row r="87" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="9"/>
+      <c r="L86" s="9"/>
+    </row>
+    <row r="87" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K87" s="9"/>
-    </row>
-    <row r="88" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J88" s="9"/>
+      <c r="L87" s="9"/>
+    </row>
+    <row r="88" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K88" s="9"/>
-    </row>
-    <row r="89" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J89" s="9"/>
+      <c r="L88" s="9"/>
+    </row>
+    <row r="89" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K89" s="9"/>
-    </row>
-    <row r="90" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J90" s="9"/>
+      <c r="L89" s="9"/>
+    </row>
+    <row r="90" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K90" s="9"/>
-    </row>
-    <row r="91" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J91" s="9"/>
+      <c r="L90" s="9"/>
+    </row>
+    <row r="91" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K91" s="9"/>
-    </row>
-    <row r="92" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J92" s="9"/>
+      <c r="L91" s="9"/>
+    </row>
+    <row r="92" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K92" s="9"/>
-    </row>
-    <row r="93" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J93" s="9"/>
+      <c r="L92" s="9"/>
+    </row>
+    <row r="93" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K93" s="9"/>
-    </row>
-    <row r="94" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J94" s="9"/>
+      <c r="L93" s="9"/>
+    </row>
+    <row r="94" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K94" s="9"/>
-    </row>
-    <row r="95" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J95" s="9"/>
+      <c r="L94" s="9"/>
+    </row>
+    <row r="95" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K95" s="9"/>
-    </row>
-    <row r="96" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J96" s="9"/>
+      <c r="L95" s="9"/>
+    </row>
+    <row r="96" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K96" s="9"/>
-    </row>
-    <row r="97" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J97" s="9"/>
+      <c r="L96" s="9"/>
+    </row>
+    <row r="97" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K97" s="9"/>
-    </row>
-    <row r="98" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J98" s="9"/>
+      <c r="L97" s="9"/>
+    </row>
+    <row r="98" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K98" s="9"/>
-    </row>
-    <row r="99" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J99" s="9"/>
+      <c r="L98" s="9"/>
+    </row>
+    <row r="99" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K99" s="9"/>
-    </row>
-    <row r="100" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J100" s="9"/>
+      <c r="L99" s="9"/>
+    </row>
+    <row r="100" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K100" s="9"/>
-    </row>
-    <row r="101" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J101" s="9"/>
+      <c r="L100" s="9"/>
+    </row>
+    <row r="101" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K101" s="9"/>
-    </row>
-    <row r="102" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J102" s="9"/>
+      <c r="L101" s="9"/>
+    </row>
+    <row r="102" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K102" s="9"/>
-    </row>
-    <row r="103" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J103" s="9"/>
+      <c r="L102" s="9"/>
+    </row>
+    <row r="103" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K103" s="9"/>
-    </row>
-    <row r="104" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J104" s="7"/>
-    </row>
-    <row r="105" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J105" s="7"/>
-    </row>
-    <row r="106" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J106" s="7"/>
-    </row>
-    <row r="107" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J107" s="7"/>
-    </row>
-    <row r="108" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J108" s="7"/>
-    </row>
-    <row r="109" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J109" s="7"/>
-    </row>
-    <row r="110" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J110" s="7"/>
-    </row>
-    <row r="111" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J111" s="7"/>
+      <c r="L103" s="9"/>
+    </row>
+    <row r="104" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K106" s="7"/>
+    </row>
+    <row r="107" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K107" s="7"/>
+    </row>
+    <row r="108" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K108" s="7"/>
+    </row>
+    <row r="109" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K109" s="7"/>
+    </row>
+    <row r="110" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K110" s="7"/>
+    </row>
+    <row r="111" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K111" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="C9:H26">
-    <sortCondition descending="1" ref="D9:D26"/>
+  <sortState ref="D9:I26">
+    <sortCondition descending="1" ref="E9:E26"/>
   </sortState>
   <mergeCells count="5">
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="25" priority="21">
-      <formula>$A4="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:D8">
-    <cfRule type="expression" dxfId="24" priority="19">
-      <formula>$A8="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="23" priority="18">
-      <formula>$A8="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="22" priority="17">
-      <formula>$A8="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="21" priority="16">
-      <formula>$A8="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="20" priority="15">
-      <formula>$A8="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="19" priority="1">
-      <formula>$A3="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="18" priority="2">
-      <formula>$A2="Even"</formula>
+  <conditionalFormatting sqref="C1:I1048576">
+    <cfRule type="expression" dxfId="16" priority="21">
+      <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -2014,18 +1917,18 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="27" t="str">
-        <f>'Detailed View'!D2</f>
+        <f>'Detailed View'!E2</f>
         <v xml:space="preserve"> | Program Lineup*</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2"/>
-      <c r="I2" s="50">
-        <f>'Detailed View'!I2:J2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="50"/>
+      <c r="I2" s="48" t="e">
+        <f>'Detailed View'!J2:K2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J2" s="48"/>
       <c r="K2" s="20"/>
       <c r="L2" s="1"/>
     </row>
@@ -2086,49 +1989,49 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
-        <f>'Detailed View'!B6:C6</f>
-        <v>0</v>
+      <c r="B6" s="46" t="e">
+        <f>'Detailed View'!C6:D6</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="25">
-        <f>'Detailed View'!D6</f>
+        <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="47">
-        <f>'Detailed View'!E6:F6</f>
-        <v>0</v>
+      <c r="E6" s="47" t="e">
+        <f>'Detailed View'!F6:G6</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F6" s="47"/>
       <c r="G6" s="25">
-        <f>'Detailed View'!G6</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="25">
+      <c r="H6" s="25">
         <f>'Detailed View'!I6</f>
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="I6" s="25">
         <f>'Detailed View'!J6</f>
         <v>0</v>
       </c>
-      <c r="K6" s="25">
+      <c r="J6" s="25">
         <f>'Detailed View'!K6</f>
         <v>0</v>
       </c>
+      <c r="K6" s="25">
+        <f>'Detailed View'!L6</f>
+        <v>0</v>
+      </c>
       <c r="L6" s="25"/>
     </row>
     <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
@@ -2150,11 +2053,11 @@
       <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
     </row>
     <row r="14" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
@@ -2176,11 +2079,11 @@
       <c r="D16" s="22"/>
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
@@ -2355,77 +2258,77 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="15" priority="19">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>$A13="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>$A10="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>$A10="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>$A10="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>$A16="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="9" priority="14">
       <formula>$A9="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="8" priority="13">
       <formula>$A17="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>$A17="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>$A17="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$A3="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2437,167 +2340,169 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:O93"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="0.28515625" style="22" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H1"/>
+    <row r="1" spans="1:15" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1"/>
-      <c r="J1" s="28"/>
-    </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="J1"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:15" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="1"/>
-      <c r="N2" s="22"/>
-    </row>
-    <row r="3" spans="1:14" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="D3" s="44" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="1"/>
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="E3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="44"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
       <c r="I3" s="44"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="N3" s="22"/>
-    </row>
-    <row r="4" spans="1:14" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="44"/>
+      <c r="M3" s="1"/>
+      <c r="O3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
-      <c r="H4" s="17"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="45"/>
+      <c r="E5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46"/>
+    <row r="6" spans="1:15" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="46"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="47"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="47"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-    </row>
-    <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10" t="s">
+      <c r="M6" s="16"/>
+    </row>
+    <row r="8" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="K8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="29"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="32"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="30"/>
+    </row>
+    <row r="10" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -2607,353 +2512,419 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
       <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J12" s="9"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
       <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J13" s="9"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
       <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
       <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J15" s="9"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
       <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="9"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
       <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="9"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
       <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J18" s="9"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
       <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J19" s="9"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
       <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J20" s="9"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
       <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J21" s="9"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
       <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J22" s="9"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
       <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J23" s="9"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
       <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J24" s="9"/>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
       <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J25" s="9"/>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
       <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J26" s="9"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
       <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J27" s="9"/>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
       <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J28" s="9"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
       <c r="K28" s="9"/>
-    </row>
-    <row r="29" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J29" s="9"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
       <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J30" s="9"/>
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
       <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J31" s="9"/>
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
       <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J32" s="9"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
       <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="9"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
       <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J34" s="9"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
       <c r="K34" s="9"/>
-    </row>
-    <row r="35" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J35" s="9"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
       <c r="K35" s="9"/>
-    </row>
-    <row r="36" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J36" s="9"/>
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
       <c r="K36" s="9"/>
-    </row>
-    <row r="37" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J37" s="9"/>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
       <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J38" s="9"/>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
       <c r="K38" s="9"/>
-    </row>
-    <row r="39" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J39" s="9"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
       <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J40" s="9"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
       <c r="K40" s="9"/>
-    </row>
-    <row r="41" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J41" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
       <c r="K41" s="9"/>
-    </row>
-    <row r="42" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="9"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
       <c r="K42" s="9"/>
-    </row>
-    <row r="43" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J43" s="9"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
       <c r="K43" s="9"/>
-    </row>
-    <row r="44" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="9"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
       <c r="K44" s="9"/>
-    </row>
-    <row r="45" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J45" s="9"/>
+      <c r="L44" s="9"/>
+    </row>
+    <row r="45" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
       <c r="K45" s="9"/>
-    </row>
-    <row r="46" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J46" s="9"/>
+      <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
       <c r="K46" s="9"/>
-    </row>
-    <row r="47" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J47" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
       <c r="K47" s="9"/>
-    </row>
-    <row r="48" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J48" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
       <c r="K48" s="9"/>
-    </row>
-    <row r="49" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J49" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
       <c r="K49" s="9"/>
-    </row>
-    <row r="50" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J50" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
       <c r="K50" s="9"/>
-    </row>
-    <row r="51" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J51" s="9"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
       <c r="K51" s="9"/>
-    </row>
-    <row r="52" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J52" s="9"/>
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
       <c r="K52" s="9"/>
-    </row>
-    <row r="53" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J53" s="9"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="24"/>
       <c r="K53" s="9"/>
-    </row>
-    <row r="54" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J54" s="9"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="24"/>
       <c r="K54" s="9"/>
-    </row>
-    <row r="55" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J55" s="9"/>
+      <c r="L54" s="9"/>
+    </row>
+    <row r="55" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
       <c r="K55" s="9"/>
-    </row>
-    <row r="56" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J56" s="9"/>
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="24"/>
       <c r="K56" s="9"/>
-    </row>
-    <row r="57" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J57" s="9"/>
+      <c r="L56" s="9"/>
+    </row>
+    <row r="57" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24"/>
       <c r="K57" s="9"/>
-    </row>
-    <row r="58" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J58" s="9"/>
+      <c r="L57" s="9"/>
+    </row>
+    <row r="58" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
       <c r="K58" s="9"/>
-    </row>
-    <row r="59" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J59" s="9"/>
+      <c r="L58" s="9"/>
+    </row>
+    <row r="59" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="24"/>
       <c r="K59" s="9"/>
-    </row>
-    <row r="60" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J60" s="9"/>
+      <c r="L59" s="9"/>
+    </row>
+    <row r="60" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24"/>
       <c r="K60" s="9"/>
-    </row>
-    <row r="61" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J61" s="9"/>
+      <c r="L60" s="9"/>
+    </row>
+    <row r="61" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
       <c r="K61" s="9"/>
-    </row>
-    <row r="62" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J62" s="9"/>
+      <c r="L61" s="9"/>
+    </row>
+    <row r="62" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24"/>
       <c r="K62" s="9"/>
-    </row>
-    <row r="63" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J63" s="9"/>
+      <c r="L62" s="9"/>
+    </row>
+    <row r="63" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
       <c r="K63" s="9"/>
-    </row>
-    <row r="64" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J64" s="9"/>
+      <c r="L63" s="9"/>
+    </row>
+    <row r="64" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="24"/>
       <c r="K64" s="9"/>
-    </row>
-    <row r="65" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J65" s="9"/>
+      <c r="L64" s="9"/>
+    </row>
+    <row r="65" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="24"/>
       <c r="K65" s="9"/>
-    </row>
-    <row r="66" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J66" s="9"/>
+      <c r="L65" s="9"/>
+    </row>
+    <row r="66" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="24"/>
       <c r="K66" s="9"/>
-    </row>
-    <row r="67" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J67" s="9"/>
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
       <c r="K67" s="9"/>
-    </row>
-    <row r="68" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J68" s="9"/>
+      <c r="L67" s="9"/>
+    </row>
+    <row r="68" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
       <c r="K68" s="9"/>
-    </row>
-    <row r="69" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J69" s="9"/>
+      <c r="L68" s="9"/>
+    </row>
+    <row r="69" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
       <c r="K69" s="9"/>
-    </row>
-    <row r="70" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J70" s="9"/>
+      <c r="L69" s="9"/>
+    </row>
+    <row r="70" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
       <c r="K70" s="9"/>
-    </row>
-    <row r="71" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J71" s="9"/>
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="24"/>
       <c r="K71" s="9"/>
-    </row>
-    <row r="72" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J72" s="9"/>
+      <c r="L71" s="9"/>
+    </row>
+    <row r="72" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="24"/>
       <c r="K72" s="9"/>
-    </row>
-    <row r="73" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J73" s="9"/>
+      <c r="L72" s="9"/>
+    </row>
+    <row r="73" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="24"/>
       <c r="K73" s="9"/>
-    </row>
-    <row r="74" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J74" s="9"/>
+      <c r="L73" s="9"/>
+    </row>
+    <row r="74" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="24"/>
       <c r="K74" s="9"/>
-    </row>
-    <row r="75" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J75" s="9"/>
+      <c r="L74" s="9"/>
+    </row>
+    <row r="75" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24"/>
       <c r="K75" s="9"/>
-    </row>
-    <row r="76" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J76" s="9"/>
+      <c r="L75" s="9"/>
+    </row>
+    <row r="76" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24"/>
       <c r="K76" s="9"/>
-    </row>
-    <row r="77" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J77" s="9"/>
+      <c r="L76" s="9"/>
+    </row>
+    <row r="77" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="24"/>
       <c r="K77" s="9"/>
-    </row>
-    <row r="78" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J78" s="9"/>
+      <c r="L77" s="9"/>
+    </row>
+    <row r="78" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="24"/>
       <c r="K78" s="9"/>
-    </row>
-    <row r="79" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="9"/>
+      <c r="L78" s="9"/>
+    </row>
+    <row r="79" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="24"/>
       <c r="K79" s="9"/>
-    </row>
-    <row r="80" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="9"/>
+      <c r="L79" s="9"/>
+    </row>
+    <row r="80" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="24"/>
       <c r="K80" s="9"/>
-    </row>
-    <row r="81" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="9"/>
+      <c r="L80" s="9"/>
+    </row>
+    <row r="81" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="24"/>
       <c r="K81" s="9"/>
-    </row>
-    <row r="82" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="9"/>
+      <c r="L81" s="9"/>
+    </row>
+    <row r="82" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="24"/>
       <c r="K82" s="9"/>
-    </row>
-    <row r="83" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="9"/>
+      <c r="L82" s="9"/>
+    </row>
+    <row r="83" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="24"/>
       <c r="K83" s="9"/>
-    </row>
-    <row r="84" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="9"/>
+      <c r="L83" s="9"/>
+    </row>
+    <row r="84" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="24"/>
       <c r="K84" s="9"/>
-    </row>
-    <row r="85" spans="10:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="9"/>
+      <c r="L84" s="9"/>
+    </row>
+    <row r="85" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="24"/>
       <c r="K85" s="9"/>
-    </row>
-    <row r="86" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="7"/>
-    </row>
-    <row r="87" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="7"/>
-    </row>
-    <row r="88" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J88" s="7"/>
-    </row>
-    <row r="89" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J89" s="7"/>
-    </row>
-    <row r="90" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J90" s="7"/>
-    </row>
-    <row r="91" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J91" s="7"/>
-    </row>
-    <row r="92" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J92" s="7"/>
-    </row>
-    <row r="93" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J93" s="7"/>
+      <c r="L85" s="9"/>
+    </row>
+    <row r="86" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K86" s="7"/>
+    </row>
+    <row r="87" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K87" s="7"/>
+    </row>
+    <row r="88" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K88" s="7"/>
+    </row>
+    <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K89" s="7"/>
+    </row>
+    <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K91" s="7"/>
+    </row>
+    <row r="92" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K93" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E3:J3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8 B4">
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>$A4="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$A2="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A3="Even"</formula>
+  <conditionalFormatting sqref="C1:K1048576">
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Merged PR 7726: PRI-20082 Fixed header layout
PRI-20082b Fixed header layout
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2146642-CCAE-4614-8C51-0E4CC814A074}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F8D507BF-5E72-41AB-91BE-D50F23395286}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
       <c r="H2" s="1"/>
       <c r="I2"/>
       <c r="J2" s="48">
-        <f>'Detailed View'!J2:K2</f>
+        <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
       <c r="K2" s="48"/>
@@ -2344,7 +2344,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2934,6 +2934,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3156,22 +3171,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3188,21 +3205,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 7735: PRI-20897 Program Lineup Report - Allocations tab
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F8D507BF-5E72-41AB-91BE-D50F23395286}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC51127F-2340-4034-9F92-958451ACD423}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,14 @@
     <cellStyle name="Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF5F8F8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -631,13 +638,13 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -783,7 +790,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -821,7 +828,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1105,7 +1112,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:K2"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1876,7 +1883,7 @@
     <mergeCell ref="J2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:I1048576">
-    <cfRule type="expression" dxfId="16" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1888,448 +1895,516 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:L105"/>
+  <dimension ref="A2:M105"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J2"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="22" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="28" style="22" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="22" customWidth="1"/>
-    <col min="13" max="16384" width="14.42578125" style="22"/>
+    <col min="1" max="1" width="14.42578125" style="22" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="28" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="22" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="22" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="22" customWidth="1"/>
+    <col min="14" max="16384" width="14.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="27" t="str">
+      <c r="D2" s="1"/>
+      <c r="E2" s="27" t="str">
         <f>'Detailed View'!E2</f>
         <v xml:space="preserve"> | Program Lineup*</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2"/>
-      <c r="I2" s="48" t="e">
-        <f>'Detailed View'!J2:K2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="D3" s="44" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2"/>
+      <c r="J2" s="48">
+        <f>'Detailed View'!J2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="48"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="E3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="44"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
       <c r="I3" s="44"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="17"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="45"/>
+      <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="F5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="e">
-        <f>'Detailed View'!C6:D6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="25">
+    <row r="6" spans="1:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="46">
+        <f>'Detailed View'!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="25">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="47" t="e">
-        <f>'Detailed View'!F6:G6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="25">
+      <c r="F6" s="47">
+        <f>'Detailed View'!F6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="47"/>
+      <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="I6" s="25">
         <f>'Detailed View'!I6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="25">
+      <c r="J6" s="25">
         <f>'Detailed View'!J6</f>
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="K6" s="25">
         <f>'Detailed View'!K6</f>
         <v>0</v>
       </c>
-      <c r="K6" s="25">
+      <c r="L6" s="25">
         <f>'Detailed View'!L6</f>
         <v>0</v>
       </c>
-      <c r="L6" s="25"/>
-    </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="M6" s="25"/>
+    </row>
+    <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="C9" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="49"/>
       <c r="D9" s="49"/>
-    </row>
-    <row r="10" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
+      <c r="E9" s="49"/>
+    </row>
+    <row r="10" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-    </row>
-    <row r="12" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
+    <row r="11" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+    </row>
+    <row r="12" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
-    </row>
-    <row r="13" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="C13" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="49"/>
       <c r="D13" s="49"/>
-    </row>
-    <row r="14" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="E14" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="36"/>
-    </row>
-    <row r="16" spans="1:12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="22"/>
+    <row r="15" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="36"/>
+    </row>
+    <row r="16" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="C17" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="50"/>
       <c r="D17" s="50"/>
-    </row>
-    <row r="18" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="3" t="s">
+      <c r="E17" s="50"/>
+    </row>
+    <row r="18" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-    </row>
-    <row r="20" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="10:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="10:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="9"/>
+    <row r="19" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="21" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+    </row>
+    <row r="24" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+    </row>
+    <row r="26" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+    </row>
+    <row r="29" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+    </row>
+    <row r="30" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+    </row>
+    <row r="31" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+    </row>
+    <row r="32" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+    </row>
+    <row r="33" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+    </row>
+    <row r="34" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+    </row>
+    <row r="35" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+    </row>
+    <row r="36" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+    </row>
+    <row r="41" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+    </row>
+    <row r="42" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+    </row>
+    <row r="43" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+    </row>
+    <row r="44" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+    </row>
+    <row r="45" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+    </row>
+    <row r="46" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="22"/>
+    </row>
+    <row r="47" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="22"/>
+    </row>
+    <row r="48" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+    </row>
+    <row r="49" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+    </row>
+    <row r="50" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+    </row>
+    <row r="51" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
+    </row>
+    <row r="52" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="22"/>
+    </row>
+    <row r="53" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="22"/>
+    </row>
+    <row r="54" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="22"/>
+    </row>
+    <row r="55" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="22"/>
+    </row>
+    <row r="56" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="22"/>
+    </row>
+    <row r="57" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="22"/>
+    </row>
+    <row r="58" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22"/>
+    </row>
+    <row r="59" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22"/>
+    </row>
+    <row r="60" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22"/>
+    </row>
+    <row r="61" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22"/>
+    </row>
+    <row r="62" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="22"/>
+    </row>
+    <row r="63" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+    </row>
+    <row r="64" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
+    </row>
+    <row r="65" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="22"/>
+    </row>
+    <row r="66" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="22"/>
+    </row>
+    <row r="67" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
+    </row>
+    <row r="68" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="22"/>
+    </row>
+    <row r="69" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+    </row>
+    <row r="70" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+    </row>
+    <row r="71" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+    </row>
+    <row r="72" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+    </row>
+    <row r="73" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="22"/>
+    </row>
+    <row r="74" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="22"/>
+    </row>
+    <row r="75" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
+    </row>
+    <row r="76" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+    </row>
+    <row r="77" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+    </row>
+    <row r="78" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+    </row>
+    <row r="79" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="22"/>
+    </row>
+    <row r="80" spans="1:1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="22"/>
+    </row>
+    <row r="81" spans="1:12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="22"/>
+    </row>
+    <row r="82" spans="1:12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="22"/>
+    </row>
+    <row r="83" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K83" s="9"/>
-    </row>
-    <row r="84" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="9"/>
+      <c r="L83" s="9"/>
+    </row>
+    <row r="84" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K84" s="9"/>
-    </row>
-    <row r="85" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="9"/>
+      <c r="L84" s="9"/>
+    </row>
+    <row r="85" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K85" s="9"/>
-    </row>
-    <row r="86" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="9"/>
+      <c r="L85" s="9"/>
+    </row>
+    <row r="86" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K86" s="9"/>
-    </row>
-    <row r="87" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="9"/>
+      <c r="L86" s="9"/>
+    </row>
+    <row r="87" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K87" s="9"/>
-    </row>
-    <row r="88" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J88" s="9"/>
+      <c r="L87" s="9"/>
+    </row>
+    <row r="88" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K88" s="9"/>
-    </row>
-    <row r="89" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J89" s="9"/>
+      <c r="L88" s="9"/>
+    </row>
+    <row r="89" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K89" s="9"/>
-    </row>
-    <row r="90" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J90" s="9"/>
+      <c r="L89" s="9"/>
+    </row>
+    <row r="90" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K90" s="9"/>
-    </row>
-    <row r="91" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J91" s="9"/>
+      <c r="L90" s="9"/>
+    </row>
+    <row r="91" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K91" s="9"/>
-    </row>
-    <row r="92" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J92" s="9"/>
+      <c r="L91" s="9"/>
+    </row>
+    <row r="92" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K92" s="9"/>
-    </row>
-    <row r="93" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J93" s="9"/>
+      <c r="L92" s="9"/>
+    </row>
+    <row r="93" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K93" s="9"/>
-    </row>
-    <row r="94" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J94" s="9"/>
+      <c r="L93" s="9"/>
+    </row>
+    <row r="94" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K94" s="9"/>
-    </row>
-    <row r="95" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J95" s="9"/>
+      <c r="L94" s="9"/>
+    </row>
+    <row r="95" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K95" s="9"/>
-    </row>
-    <row r="96" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J96" s="9"/>
+      <c r="L95" s="9"/>
+    </row>
+    <row r="96" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K96" s="9"/>
-    </row>
-    <row r="97" spans="10:11" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J97" s="9"/>
+      <c r="L96" s="9"/>
+    </row>
+    <row r="97" spans="11:12" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K97" s="9"/>
-    </row>
-    <row r="98" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J99" s="7"/>
-    </row>
-    <row r="100" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J101" s="7"/>
-    </row>
-    <row r="102" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J102" s="7"/>
-    </row>
-    <row r="103" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J103" s="7"/>
-    </row>
-    <row r="104" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J104" s="7"/>
-    </row>
-    <row r="105" spans="10:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J105" s="7"/>
+      <c r="L97" s="9"/>
+    </row>
+    <row r="98" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K98" s="7"/>
+    </row>
+    <row r="99" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K99" s="7"/>
+    </row>
+    <row r="100" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K100" s="7"/>
+    </row>
+    <row r="101" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K101" s="7"/>
+    </row>
+    <row r="102" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K102" s="7"/>
+    </row>
+    <row r="103" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K103" s="7"/>
+    </row>
+    <row r="104" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="11:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K105" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="15" priority="19">
-      <formula>$A4="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="14" priority="6">
-      <formula>$A13="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>$A10="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>$A10="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>$A10="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>$A16="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="9" priority="14">
-      <formula>$A9="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="8" priority="13">
-      <formula>$A17="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="7" priority="12">
-      <formula>$A17="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="6" priority="11">
-      <formula>$A17="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$A3="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="4" priority="7">
-      <formula>$A14="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="3" priority="9">
-      <formula>$A14="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>$A14="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$A2="Even"</formula>
+  <conditionalFormatting sqref="C1:E1048576">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -2923,7 +2998,7 @@
     <mergeCell ref="E3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:K1048576">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2934,21 +3009,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3171,24 +3231,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3205,4 +3263,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 8916: BP1-501 : Program lineup - Display allocations to 2 decimal places
CR Task : https://jira.crossmw.com/browse/BP1-633
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC51127F-2340-4034-9F92-958451ACD423}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA89CAF-C7EF-4B81-A7B3-67F2103E0D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="435" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
     <sheet name="Allocations" sheetId="6" r:id="rId2"/>
     <sheet name="Detailed View" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mgMtMfamHb1jVya39tpwhGUN2dNvA=="/>
     </ext>
@@ -429,16 +437,10 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -470,6 +472,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -477,112 +485,7 @@
     <cellStyle name="Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -638,13 +541,13 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1145,24 +1048,24 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="48">
+      <c r="J2" s="46">
         <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="48"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1182,10 +1085,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1210,20 +1113,20 @@
       </c>
     </row>
     <row r="6" spans="2:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="46">
+      <c r="C6" s="44">
         <f>'Detailed View'!C6:D6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="25">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="45">
         <f>'Detailed View'!F6:G6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -1271,13 +1174,13 @@
     </row>
     <row r="9" spans="2:13" s="24" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9"/>
-      <c r="C9" s="41"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="32"/>
-      <c r="E9" s="42"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
-      <c r="I9" s="43"/>
+      <c r="I9" s="41"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -1872,7 +1775,7 @@
       <c r="K111" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="D9:I26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D9:I26">
     <sortCondition descending="1" ref="E9:E26"/>
   </sortState>
   <mergeCells count="5">
@@ -1883,7 +1786,7 @@
     <mergeCell ref="J2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:I1048576">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="2" priority="21">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1932,24 +1835,24 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="48">
+      <c r="J2" s="46">
         <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="48"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1969,10 +1872,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1997,20 +1900,20 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="46">
+      <c r="C6" s="44">
         <f>'Detailed View'!C6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="25">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="45">
         <f>'Detailed View'!F6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -2036,11 +1939,11 @@
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
     </row>
     <row r="10" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
@@ -2054,9 +1957,9 @@
     </row>
     <row r="11" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="49"/>
     </row>
     <row r="12" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
@@ -2066,11 +1969,11 @@
     </row>
     <row r="13" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
     </row>
     <row r="14" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
@@ -2086,7 +1989,7 @@
       <c r="A15" s="22"/>
       <c r="C15" s="35"/>
       <c r="D15" s="32"/>
-      <c r="E15" s="36"/>
+      <c r="E15" s="50"/>
     </row>
     <row r="16" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -2096,11 +1999,11 @@
     </row>
     <row r="17" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
     </row>
     <row r="18" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
@@ -2114,9 +2017,9 @@
     </row>
     <row r="19" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="49"/>
     </row>
     <row r="20" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
@@ -2403,7 +2306,7 @@
     <mergeCell ref="F6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="expression" dxfId="0" priority="19">
+    <cfRule type="expression" dxfId="1" priority="19">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2456,22 +2359,22 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
       <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2479,12 +2382,12 @@
     </row>
     <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
@@ -2492,10 +2395,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="19" t="s">
         <v>13</v>
       </c>
@@ -2520,11 +2423,11 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -2998,7 +2901,7 @@
     <mergeCell ref="E3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:K1048576">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3009,6 +2912,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3231,12 +3140,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3247,6 +3150,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3265,15 +3177,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Merged PR 9746: BP-65 Program Lineup Report - Integrate Multiple Spot Lengths
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA89CAF-C7EF-4B81-A7B3-67F2103E0D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C836EE8-A864-422E-B4B4-DAECA17DB3B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="435" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,16 +17,8 @@
     <sheet name="Allocations" sheetId="6" r:id="rId2"/>
     <sheet name="Detailed View" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mgMtMfamHb1jVya39tpwhGUN2dNvA=="/>
     </ext>
@@ -35,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>DMA</t>
   </si>
@@ -110,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve"> | Program Lineup*</t>
+  </si>
+  <si>
+    <t>Allocation by Spot Length</t>
   </si>
 </sst>
 </file>
@@ -453,6 +448,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -472,12 +473,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -1048,24 +1043,24 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="46">
+      <c r="J2" s="48">
         <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="46"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1085,10 +1080,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1113,20 +1108,20 @@
       </c>
     </row>
     <row r="6" spans="2:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="44">
+      <c r="C6" s="46">
         <f>'Detailed View'!C6:D6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="25">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="47">
         <f>'Detailed View'!F6:G6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="45"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -1775,7 +1770,7 @@
       <c r="K111" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D9:I26">
+  <sortState ref="D9:I26">
     <sortCondition descending="1" ref="E9:E26"/>
   </sortState>
   <mergeCells count="5">
@@ -1802,7 +1797,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1835,24 +1830,24 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="46">
+      <c r="J2" s="48">
         <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="46"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1872,10 +1867,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1900,20 +1895,20 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="44">
+      <c r="C6" s="46">
         <f>'Detailed View'!C6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="25">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="47">
         <f>'Detailed View'!F6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="45"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -1939,11 +1934,11 @@
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
@@ -1959,7 +1954,7 @@
       <c r="A11" s="22"/>
       <c r="C11" s="38"/>
       <c r="D11" s="37"/>
-      <c r="E11" s="49"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
@@ -1969,11 +1964,11 @@
     </row>
     <row r="13" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
     </row>
     <row r="14" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
@@ -1989,7 +1984,7 @@
       <c r="A15" s="22"/>
       <c r="C15" s="35"/>
       <c r="D15" s="32"/>
-      <c r="E15" s="50"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -1999,11 +1994,11 @@
     </row>
     <row r="17" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
     </row>
     <row r="18" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
@@ -2019,19 +2014,34 @@
       <c r="A19" s="22"/>
       <c r="C19" s="36"/>
       <c r="D19" s="37"/>
-      <c r="E19" s="49"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
     </row>
     <row r="21" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-    </row>
-    <row r="22" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+    </row>
+    <row r="22" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-    </row>
-    <row r="23" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="42"/>
     </row>
     <row r="24" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
@@ -2295,7 +2305,8 @@
       <c r="K105" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C13:E13"/>
@@ -2359,22 +2370,22 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
       <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2382,12 +2393,12 @@
     </row>
     <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
@@ -2395,10 +2406,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="19" t="s">
         <v>13</v>
       </c>
@@ -2423,11 +2434,11 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -2918,6 +2929,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3140,15 +3160,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
   <ds:schemaRefs>
@@ -3159,6 +3170,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3175,12 +3194,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>